<commit_message>
Added Documentation for Helcaraxe.py
</commit_message>
<xml_diff>
--- a/RESULTS/evaluation_table_test_Fobs_commented.xlsx
+++ b/RESULTS/evaluation_table_test_Fobs_commented.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/My Passport/Helcaraxe/ARM_env/RESULTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristophernolte/Documents/GitHub/helcaraxe/RESULTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF059B-872E-0C42-91CD-A075C58C65B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8DBCC5-51B6-1D4A-B415-4A4AEFA8BF6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1425">
   <si>
     <t>names</t>
   </si>
@@ -4259,9 +4259,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>small</t>
   </si>
   <si>
     <t>broad, covered</t>
@@ -4304,7 +4301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4337,6 +4334,14 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4377,7 +4382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4387,6 +4392,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4691,8 +4699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -4740,7 +4748,7 @@
         <v>0.97489424422383308</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4760,7 +4768,7 @@
         <v>0.98968708235770464</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4780,7 +4788,7 @@
         <v>0.99347094399854541</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4800,7 +4808,7 @@
         <v>0.56407326459884644</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4820,144 +4828,144 @@
         <v>0.98008422739803791</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>570</v>
+        <v>769</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>574</v>
+        <v>773</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>6.3417511992156514E-3</v>
+        <v>8.6089685559272766E-2</v>
       </c>
       <c r="E7" s="4">
-        <v>0.99365824880078435</v>
+        <v>0.91391031444072723</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>773</v>
+        <v>896</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>8.6089685559272766E-2</v>
+        <v>0.32431188225746149</v>
       </c>
       <c r="E8" s="4">
-        <v>0.91391031444072723</v>
+        <v>0.67568811774253845</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>892</v>
+        <v>972</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>896</v>
+        <v>976</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4">
-        <v>0.32431188225746149</v>
+        <v>0.22781865298748019</v>
       </c>
       <c r="E9" s="4">
-        <v>0.67568811774253845</v>
+        <v>0.77218134701251984</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>972</v>
+        <v>1123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>976</v>
+        <v>1127</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="4">
-        <v>0.22781865298748019</v>
+        <v>1.977664884179831E-3</v>
       </c>
       <c r="E10" s="4">
-        <v>0.77218134701251984</v>
+        <v>0.99802233511582017</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>1123</v>
+        <v>1195</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1127</v>
+        <v>1199</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4">
-        <v>1.977664884179831E-3</v>
+        <v>1.9400174496695399E-3</v>
       </c>
       <c r="E11" s="4">
-        <v>0.99802233511582017</v>
+        <v>0.99805998255033046</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>1195</v>
+        <v>1362</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1199</v>
+        <v>1366</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>1.9400174496695399E-3</v>
+        <v>0.29677078127861017</v>
       </c>
       <c r="E12" s="4">
-        <v>0.99805998255033046</v>
+        <v>0.70322921872138977</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1362</v>
+        <v>297</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1366</v>
+        <v>301</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>0.29677078127861017</v>
+        <v>0.6921268105506897</v>
       </c>
       <c r="E13" s="4">
-        <v>0.70322921872138977</v>
+        <v>0.6921268105506897</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>1415</v>
@@ -4965,425 +4973,413 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>297</v>
+        <v>357</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>0.6921268105506897</v>
+        <v>0.5227246880531311</v>
       </c>
       <c r="E14" s="4">
-        <v>0.6921268105506897</v>
+        <v>0.5227246880531311</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>357</v>
+        <v>527</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>361</v>
+        <v>531</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>0.5227246880531311</v>
+        <v>7.1872945409268141E-4</v>
       </c>
       <c r="E15" s="4">
-        <v>0.5227246880531311</v>
+        <v>7.1872945409268141E-4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>1241</v>
+        <v>611</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1245</v>
+        <v>615</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4">
-        <v>2.489242004230618E-3</v>
+        <v>4.3291077599860728E-4</v>
       </c>
       <c r="E16" s="4">
-        <v>0.99751075799576938</v>
+        <v>0.99956708922400139</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>527</v>
+        <v>1073</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>531</v>
+        <v>1077</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="4">
-        <v>7.1872945409268141E-4</v>
+        <v>1.648784382268786E-3</v>
       </c>
       <c r="E17" s="4">
-        <v>0.99928127054590732</v>
+        <v>0.99835121561773121</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>611</v>
+        <v>923</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>615</v>
+        <v>927</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
       </c>
       <c r="D18" s="4">
-        <v>4.3291077599860728E-4</v>
+        <v>0.1190106272697449</v>
       </c>
       <c r="E18" s="4">
-        <v>0.99956708922400139</v>
+        <v>0.88098937273025513</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>1073</v>
+        <v>1042</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1077</v>
+        <v>1046</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="4">
-        <v>1.648784382268786E-3</v>
+        <v>0.37290817499160772</v>
       </c>
       <c r="E19" s="4">
-        <v>0.99835121561773121</v>
+        <v>0.62709182500839233</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1420</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>133</v>
+        <v>811</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>137</v>
+        <v>815</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="D20" s="4">
-        <v>1.37466040905565E-3</v>
+        <v>0.138919472694397</v>
       </c>
       <c r="E20" s="4">
-        <v>0.99862533959094435</v>
+        <v>0.86108052730560303</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1413</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>923</v>
+        <v>1272</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>927</v>
+        <v>1276</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>0.1190106272697449</v>
+        <v>8.8452029740437865E-4</v>
       </c>
       <c r="E21" s="4">
-        <v>0.88098937273025513</v>
+        <v>0.99911547970259562</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>1042</v>
+        <v>417</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1046</v>
+        <v>421</v>
       </c>
       <c r="C22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>0.37290817499160772</v>
+        <v>0.52431172132492065</v>
       </c>
       <c r="E22" s="4">
-        <v>0.62709182500839233</v>
+        <v>0.52431172132492065</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1425</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>811</v>
+        <v>665</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>815</v>
+        <v>669</v>
       </c>
       <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="D23" s="4">
-        <v>0.138919472694397</v>
+        <v>5.2908904850482941E-2</v>
       </c>
       <c r="E23" s="4">
-        <v>0.86108052730560303</v>
+        <v>0.94709109514951706</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>1272</v>
+        <v>666</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1276</v>
+        <v>670</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>8.8452029740437865E-4</v>
+        <v>1.4823236269876361E-3</v>
       </c>
       <c r="E24" s="4">
-        <v>0.99911547970259562</v>
+        <v>0.99851767637301236</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>417</v>
+        <v>1121</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>421</v>
+        <v>1125</v>
       </c>
       <c r="C25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="4">
-        <v>0.52431172132492065</v>
+        <v>1.274482253938913E-2</v>
       </c>
       <c r="E25" s="4">
-        <v>0.52431172132492065</v>
+        <v>0.98725517746061087</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>665</v>
+        <v>309</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>669</v>
+        <v>313</v>
       </c>
       <c r="C26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>5.2908904850482941E-2</v>
+        <v>0.78195148706436157</v>
       </c>
       <c r="E26" s="4">
-        <v>0.94709109514951706</v>
+        <v>0.78195148706436157</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>666</v>
+        <v>532</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>670</v>
+        <v>536</v>
       </c>
       <c r="C27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>1.4823236269876361E-3</v>
+        <v>0.8638160228729248</v>
       </c>
       <c r="E27" s="4">
-        <v>0.99851767637301236</v>
+        <v>0.8638160228729248</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>981</v>
+        <v>810</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>985</v>
+        <v>814</v>
       </c>
       <c r="C28" s="4">
         <v>1</v>
       </c>
       <c r="D28" s="4">
-        <v>2.2985241375863552E-3</v>
+        <v>0.27379903197288508</v>
       </c>
       <c r="E28" s="4">
-        <v>0.99770147586241364</v>
+        <v>0.72620096802711487</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>1121</v>
+        <v>812</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1125</v>
+        <v>816</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
       </c>
       <c r="D29" s="4">
-        <v>1.274482253938913E-2</v>
+        <v>0.25301164388656622</v>
       </c>
       <c r="E29" s="4">
-        <v>0.98725517746061087</v>
+        <v>0.74698835611343384</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>309</v>
+        <v>1112</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>313</v>
+        <v>1116</v>
       </c>
       <c r="C30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="4">
-        <v>0.78195148706436157</v>
+        <v>1.319265551865101E-2</v>
       </c>
       <c r="E30" s="4">
-        <v>0.78195148706436157</v>
+        <v>0.98680734448134899</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>532</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.8638160228729248</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0.8638160228729248</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>1417</v>
+      <c r="A31" s="5">
+        <v>570</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6.3417511992156514E-3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6.3417511992156514E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>810</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>814</v>
-      </c>
-      <c r="C32" s="4">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.27379903197288508</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0.72620096802711487</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>812</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>816</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0.25301164388656622</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0.74698835611343384</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>1112</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>1116</v>
-      </c>
-      <c r="C34" s="4">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1.319265551865101E-2</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0.98680734448134899</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>1241</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.489242004230618E-3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.489242004230618E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>133</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.37466040905565E-3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.37466040905565E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>981</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2.2985241375863552E-3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2.2985241375863552E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>0</v>
       </c>
@@ -5400,7 +5396,7 @@
         <v>3.8378481986001128E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -5417,7 +5413,7 @@
         <v>2.9180763522163028E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -5434,7 +5430,7 @@
         <v>8.9417886920273304E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -5451,7 +5447,7 @@
         <v>4.5866824802942569E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -5468,7 +5464,7 @@
         <v>2.606455702334642E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>5</v>
       </c>
@@ -5485,7 +5481,7 @@
         <v>8.8007398881018162E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>6</v>
       </c>
@@ -5502,7 +5498,7 @@
         <v>1.7791043501347299E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>7</v>
       </c>
@@ -5519,7 +5515,7 @@
         <v>5.1024137064814568E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>8</v>
       </c>
@@ -5536,7 +5532,7 @@
         <v>1.106908661313355E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -5553,7 +5549,7 @@
         <v>3.442822489887476E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -5570,7 +5566,7 @@
         <v>1.1738172033801671E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>11</v>
       </c>
@@ -5587,7 +5583,7 @@
         <v>4.378635436296463E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -5604,7 +5600,7 @@
         <v>7.460978627204895E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>13</v>
       </c>
@@ -7142,13 +7138,13 @@
         <v>107</v>
       </c>
       <c r="C138" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D138" s="1">
         <v>0.96003758907318115</v>
       </c>
       <c r="E138" s="1">
-        <v>3.9962410926818848E-2</v>
+        <v>0.96003758907318115</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -17852,13 +17848,13 @@
         <v>750</v>
       </c>
       <c r="C768" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D768" s="1">
         <v>0.56404823064804077</v>
       </c>
       <c r="E768" s="1">
-        <v>0.43595176935195917</v>
+        <v>0.56404823064804077</v>
       </c>
     </row>
     <row r="769" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>